<commit_message>
bert + mean_std, excel results with mean and std
</commit_message>
<xml_diff>
--- a/summarization_textrank_results.xlsx
+++ b/summarization_textrank_results.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q14"/>
+  <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,6 +434,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="n">
         <v>0</v>
       </c>
@@ -484,7 +489,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>add_kg_info</t>
         </is>
@@ -571,7 +576,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+      <c r="A3" t="inlineStr">
         <is>
           <t>wiki_usage</t>
         </is>
@@ -658,7 +663,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
+      <c r="A4" t="inlineStr">
         <is>
           <t>kind_summ</t>
         </is>
@@ -745,7 +750,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
+      <c r="A5" t="inlineStr">
         <is>
           <t>counting</t>
         </is>
@@ -832,7 +837,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
+      <c r="A6" t="inlineStr">
         <is>
           <t>ROUGE-1</t>
         </is>
@@ -887,7 +892,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="inlineStr">
+      <c r="A7" t="inlineStr">
         <is>
           <t>ROUGE-2</t>
         </is>
@@ -942,7 +947,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="inlineStr">
+      <c r="A8" t="inlineStr">
         <is>
           <t>ROUGE-L</t>
         </is>
@@ -997,7 +1002,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="inlineStr">
+      <c r="A9" t="inlineStr">
         <is>
           <t>BLEU</t>
         </is>
@@ -1052,7 +1057,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="inlineStr">
+      <c r="A10" t="inlineStr">
         <is>
           <t>BERT Precision</t>
         </is>
@@ -1107,7 +1112,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="inlineStr">
+      <c r="A11" t="inlineStr">
         <is>
           <t>BERT Recall</t>
         </is>
@@ -1162,7 +1167,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
+      <c r="A12" t="inlineStr">
         <is>
           <t>BERT F1</t>
         </is>
@@ -1217,7 +1222,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="inlineStr">
+      <c r="A13" t="inlineStr">
         <is>
           <t>Cosine Similarity</t>
         </is>
@@ -1272,7 +1277,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="inlineStr">
+      <c r="A14" t="inlineStr">
         <is>
           <t>Spent Time</t>
         </is>
@@ -1324,6 +1329,116 @@
       </c>
       <c r="Q14" t="n">
         <v>0.01</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>mean</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.4932613673042583</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.5382312831640398</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.4932613673042583</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.5371201720529286</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.4921502561931472</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.5382312831640398</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.4932613673042583</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.5382312831640398</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.4921502561931472</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.5371201720529286</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.4932613673042583</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0.5382312831640398</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0.4932613673042583</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0.5382312831640398</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0.4921502561931472</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>0.5382312831640398</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>std</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0.3627495052232896</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.3487818395416044</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.3627495052232896</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.3506857010387602</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.3644262175929625</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.3487818395416044</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.3627495052232896</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.3487818395416044</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.3644262175929625</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0.3506857010387602</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0.3627495052232896</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0.3487818395416044</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0.3627495052232896</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0.3487818395416044</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0.3644262175929625</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>0.3487818395416044</v>
       </c>
     </row>
   </sheetData>

</xml_diff>